<commit_message>
Adding in code to put nurses in the database, added in the bulk uploader module to the Nurse model, fixing up spreadsheet fixtures
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/spreadsheets/basic_spreadsheet.xlsx
+++ b/spec/fixtures/files/spreadsheets/basic_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Number of Weeks Off</t>
+  </si>
+  <si>
+    <t>nurse 3</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -446,6 +449,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>